<commit_message>
Implemento parcial dos 3 casos de teste e implementação da massa de dados nos testes da pesquisar pela lupa e pela home page
</commit_message>
<xml_diff>
--- a/src/main/java/arquivos/bancoDados.xlsx
+++ b/src/main/java/arquivos/bancoDados.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saulo.silva\Downloads\hub_TDD_BDD-master\hub_TDD_BDD-master\src\main\java\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391A1592-F41E-4292-9EE5-6D4BA0F41BD5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02395089-73B4-42FE-9385-235893D0A038}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D514BC7B-BE3F-4BB9-9548-BB59BDF80586}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{D514BC7B-BE3F-4BB9-9548-BB59BDF80586}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>Usuario</t>
   </si>
@@ -139,13 +141,55 @@
   </si>
   <si>
     <t>Criou o cadastro com sucesso</t>
+  </si>
+  <si>
+    <t>mice</t>
+  </si>
+  <si>
+    <t>headphones</t>
+  </si>
+  <si>
+    <t>tablets</t>
+  </si>
+  <si>
+    <t>speakers</t>
+  </si>
+  <si>
+    <t>HP ENVY - 17T TOUCH LAPTOP</t>
+  </si>
+  <si>
+    <t>Logitech USB Headset H390</t>
+  </si>
+  <si>
+    <t>HP Elite x2 1011 G1 Tablet</t>
+  </si>
+  <si>
+    <t>HP Roar Plus Wireless Speaker</t>
+  </si>
+  <si>
+    <t>laptops</t>
+  </si>
+  <si>
+    <t>pesquisa</t>
+  </si>
+  <si>
+    <t>nome produto</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>miceImg</t>
+  </si>
+  <si>
+    <t>nome</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +201,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -183,10 +242,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -504,7 +565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B9136E-0E6B-411A-8662-0AE91BD9A6DE}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -653,4 +714,113 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF751C6D-0313-48F7-A015-FFF3B2048B34}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E5E720D-4A25-4E28-8EF2-3AA0EC049590}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finalizei os testes de cadastro
</commit_message>
<xml_diff>
--- a/src/main/java/arquivos/bancoDados.xlsx
+++ b/src/main/java/arquivos/bancoDados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saulo.silva\Downloads\hub_TDD_BDD-master\hub_TDD_BDD-master\src\main\java\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02395089-73B4-42FE-9385-235893D0A038}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAE99B5-669F-4A41-98B9-494B19A2B772}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{D514BC7B-BE3F-4BB9-9548-BB59BDF80586}"/>
+    <workbookView xWindow="2130" yWindow="1130" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{D514BC7B-BE3F-4BB9-9548-BB59BDF80586}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>Usuario</t>
   </si>
@@ -155,9 +155,6 @@
     <t>speakers</t>
   </si>
   <si>
-    <t>HP ENVY - 17T TOUCH LAPTOP</t>
-  </si>
-  <si>
     <t>Logitech USB Headset H390</t>
   </si>
   <si>
@@ -182,7 +179,49 @@
     <t>miceImg</t>
   </si>
   <si>
-    <t>nome</t>
+    <t>Logitech G502 Proteus Core</t>
+  </si>
+  <si>
+    <t>campo</t>
+  </si>
+  <si>
+    <t>produto</t>
+  </si>
+  <si>
+    <t>HP Z4000 Wireless Mouse</t>
+  </si>
+  <si>
+    <t>HP USB 3 Button Optical Mouse</t>
+  </si>
+  <si>
+    <t>HP Z3200 Wireless Mouse</t>
+  </si>
+  <si>
+    <t>HP Z3600 Wireless Mouse</t>
+  </si>
+  <si>
+    <t>HP Z8000 Bluetooth Mouse</t>
+  </si>
+  <si>
+    <t>Kensington Orbit 72337 Trackball with Scroll Ring</t>
+  </si>
+  <si>
+    <t>Kensington Orbit 72352 Trackball</t>
+  </si>
+  <si>
+    <t>Microsoft Sculpt Touch Mouse</t>
+  </si>
+  <si>
+    <t>Tablets</t>
+  </si>
+  <si>
+    <t>tabletsImg</t>
+  </si>
+  <si>
+    <t>HP Pro Tablet 608 G1</t>
+  </si>
+  <si>
+    <t>HP ZBook 17 G2 Mobile Workstation</t>
   </si>
 </sst>
 </file>
@@ -720,38 +759,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF751C6D-0313-48F7-A015-FFF3B2048B34}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="22.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2">
-        <v>7</v>
+        <v>43</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
@@ -761,7 +795,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -769,7 +803,7 @@
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -777,7 +811,7 @@
         <v>38</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -785,38 +819,100 @@
         <v>39</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E5E720D-4A25-4E28-8EF2-3AA0EC049590}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B7" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C3" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C4" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C5" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C6" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C7" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C8" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C10" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tirando thread sleep e colocando os casos de falha
</commit_message>
<xml_diff>
--- a/src/main/java/arquivos/bancoDados.xlsx
+++ b/src/main/java/arquivos/bancoDados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saulo.silva\Downloads\hub_TDD_BDD-master\hub_TDD_BDD-master\src\main\java\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAE99B5-669F-4A41-98B9-494B19A2B772}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E8E5EE-DA91-4A9B-81F1-64020E1DB3B8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="1130" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{D514BC7B-BE3F-4BB9-9548-BB59BDF80586}"/>
+    <workbookView xWindow="2840" yWindow="840" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{D514BC7B-BE3F-4BB9-9548-BB59BDF80586}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>Usuario</t>
   </si>
@@ -173,12 +173,6 @@
     <t>nome produto</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>miceImg</t>
-  </si>
-  <si>
     <t>Logitech G502 Proteus Core</t>
   </si>
   <si>
@@ -215,13 +209,16 @@
     <t>Tablets</t>
   </si>
   <si>
-    <t>tabletsImg</t>
-  </si>
-  <si>
     <t>HP Pro Tablet 608 G1</t>
   </si>
   <si>
     <t>HP ZBook 17 G2 Mobile Workstation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MICE </t>
+  </si>
+  <si>
+    <t>apple</t>
   </si>
 </sst>
 </file>
@@ -757,7 +754,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF751C6D-0313-48F7-A015-FFF3B2048B34}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -785,7 +782,7 @@
         <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
@@ -818,8 +815,13 @@
       <c r="A7" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -832,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E5E720D-4A25-4E28-8EF2-3AA0EC049590}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B7" sqref="B6:B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -844,75 +846,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>47</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C4" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C5" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C6" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C7" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C8" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C9" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C10" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Organizando a page Object e o teste de falha da pesquisa pela home
</commit_message>
<xml_diff>
--- a/src/main/java/arquivos/bancoDados.xlsx
+++ b/src/main/java/arquivos/bancoDados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saulo.silva\Downloads\hub_TDD_BDD-master\hub_TDD_BDD-master\src\main\java\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E8E5EE-DA91-4A9B-81F1-64020E1DB3B8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C165C3ED-F3F8-45D3-9814-221E5E3F25EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="840" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{D514BC7B-BE3F-4BB9-9548-BB59BDF80586}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D514BC7B-BE3F-4BB9-9548-BB59BDF80586}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
   <si>
     <t>Usuario</t>
   </si>
@@ -137,12 +137,6 @@
     <t>(11)12345</t>
   </si>
   <si>
-    <t>saulosjss33</t>
-  </si>
-  <si>
-    <t>Criou o cadastro com sucesso</t>
-  </si>
-  <si>
     <t>mice</t>
   </si>
   <si>
@@ -219,6 +213,15 @@
   </si>
   <si>
     <t>apple</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>One upper letter required</t>
+  </si>
+  <si>
+    <t>saulosjs25</t>
   </si>
 </sst>
 </file>
@@ -601,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B9136E-0E6B-411A-8662-0AE91BD9A6DE}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -616,7 +619,7 @@
     <col min="7" max="7" width="15" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="9.6328125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.7265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
@@ -662,7 +665,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -698,7 +701,7 @@
         <v>33</v>
       </c>
       <c r="M2" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -737,6 +740,9 @@
       </c>
       <c r="L3" t="s">
         <v>33</v>
+      </c>
+      <c r="M3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
@@ -756,72 +762,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF751C6D-0313-48F7-A015-FFF3B2048B34}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.26953125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -840,74 +846,74 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="41.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C3" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C5" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C6" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C7" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C8" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C9" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C10" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>